<commit_message>
Added one more detail to analysis of trade suggestions
</commit_message>
<xml_diff>
--- a/docs/proposed_trades.xlsx
+++ b/docs/proposed_trades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\mcp\mlbchat\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9F6327-E5AB-429A-A630-90AE57FE2EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DE7783-2775-4517-85CC-B43B058AB00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="86" yWindow="1020" windowWidth="32614" windowHeight="15969" activeTab="1" xr2:uid="{F042A249-47C6-4134-B927-1CE0688B40C2}"/>
   </bookViews>
@@ -1147,9 +1147,6 @@
     <t>Bobby Miller, Nick Nastrini, Landon Knack</t>
   </si>
   <si>
-    <t>Michael Grove, Nick Frasso, Any Pages</t>
-  </si>
-  <si>
     <t>Gavin Stone, Jack Dreyer</t>
   </si>
   <si>
@@ -1424,6 +1421,9 @@
   </si>
   <si>
     <t>Richard Fitts</t>
+  </si>
+  <si>
+    <t>Michael Grove, Nick Frasso, Andy Pages</t>
   </si>
 </sst>
 </file>
@@ -9662,8 +9662,8 @@
   <dimension ref="A1:K177"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L74" sqref="L74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -11357,7 +11357,7 @@
         <v>22</v>
       </c>
       <c r="E73" t="s">
-        <v>370</v>
+        <v>462</v>
       </c>
       <c r="G73" t="s">
         <v>58</v>
@@ -11380,7 +11380,7 @@
         <v>22</v>
       </c>
       <c r="E74" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G74" t="s">
         <v>108</v>
@@ -11403,13 +11403,13 @@
         <v>38</v>
       </c>
       <c r="E75" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G75" t="s">
         <v>64</v>
       </c>
       <c r="I75" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.4">
@@ -11432,7 +11432,7 @@
         <v>119</v>
       </c>
       <c r="I76" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.4">
@@ -11455,7 +11455,7 @@
         <v>46</v>
       </c>
       <c r="I77" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.4">
@@ -11492,7 +11492,7 @@
         <v>108</v>
       </c>
       <c r="E79" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G79" t="s">
         <v>29</v>
@@ -11518,7 +11518,7 @@
         <v>57</v>
       </c>
       <c r="I80" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.4">
@@ -11541,7 +11541,7 @@
         <v>57</v>
       </c>
       <c r="I81" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.4">
@@ -11558,7 +11558,7 @@
         <v>108</v>
       </c>
       <c r="E82" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G82" t="s">
         <v>57</v>
@@ -11584,7 +11584,7 @@
         <v>45</v>
       </c>
       <c r="I83" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.4">
@@ -11607,7 +11607,7 @@
         <v>67</v>
       </c>
       <c r="I84" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.4">
@@ -11624,13 +11624,13 @@
         <v>171</v>
       </c>
       <c r="E85" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G85" t="s">
         <v>119</v>
       </c>
       <c r="I85" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.4">
@@ -11653,7 +11653,7 @@
         <v>29</v>
       </c>
       <c r="I86" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.4">
@@ -11676,7 +11676,7 @@
         <v>14</v>
       </c>
       <c r="I87" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.4">
@@ -11693,13 +11693,13 @@
         <v>171</v>
       </c>
       <c r="E88" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G88" t="s">
         <v>31</v>
       </c>
       <c r="I88" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.4">
@@ -11739,7 +11739,7 @@
         <v>119</v>
       </c>
       <c r="E90" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="G90" t="s">
         <v>79</v>
@@ -11785,7 +11785,7 @@
         <v>58</v>
       </c>
       <c r="I92" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.4">
@@ -11822,7 +11822,7 @@
         <v>119</v>
       </c>
       <c r="E94" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G94" t="s">
         <v>38</v>
@@ -11845,7 +11845,7 @@
         <v>119</v>
       </c>
       <c r="E95" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G95" t="s">
         <v>35</v>
@@ -11868,7 +11868,7 @@
         <v>119</v>
       </c>
       <c r="E96" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G96" t="s">
         <v>120</v>
@@ -11891,13 +11891,13 @@
         <v>24</v>
       </c>
       <c r="E97" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G97" t="s">
         <v>45</v>
       </c>
       <c r="I97" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.4">
@@ -11920,7 +11920,7 @@
         <v>77</v>
       </c>
       <c r="I98" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.4">
@@ -11937,7 +11937,7 @@
         <v>24</v>
       </c>
       <c r="E99" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G99" t="s">
         <v>14</v>
@@ -11960,7 +11960,7 @@
         <v>24</v>
       </c>
       <c r="E100" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G100" t="s">
         <v>31</v>
@@ -11983,13 +11983,13 @@
         <v>24</v>
       </c>
       <c r="E101" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G101" t="s">
         <v>57</v>
       </c>
       <c r="I101" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.4">
@@ -12012,7 +12012,7 @@
         <v>38</v>
       </c>
       <c r="I102" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.4">
@@ -12029,13 +12029,13 @@
         <v>24</v>
       </c>
       <c r="E103" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G103" t="s">
         <v>46</v>
       </c>
       <c r="I103" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.4">
@@ -12052,13 +12052,13 @@
         <v>64</v>
       </c>
       <c r="E104" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G104" t="s">
         <v>56</v>
       </c>
       <c r="I104" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.4">
@@ -12075,13 +12075,13 @@
         <v>64</v>
       </c>
       <c r="E105" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G105" t="s">
         <v>29</v>
       </c>
       <c r="I105" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.4">
@@ -12098,13 +12098,13 @@
         <v>64</v>
       </c>
       <c r="E106" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G106" t="s">
         <v>38</v>
       </c>
       <c r="I106" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.4">
@@ -12121,13 +12121,13 @@
         <v>64</v>
       </c>
       <c r="E107" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="G107" t="s">
         <v>38</v>
       </c>
       <c r="I107" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.4">
@@ -12144,13 +12144,13 @@
         <v>102</v>
       </c>
       <c r="E108" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G108" t="s">
         <v>311</v>
       </c>
       <c r="I108" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.4">
@@ -12173,7 +12173,7 @@
         <v>79</v>
       </c>
       <c r="I109" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.4">
@@ -12190,13 +12190,13 @@
         <v>102</v>
       </c>
       <c r="E110" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G110" t="s">
         <v>311</v>
       </c>
       <c r="I110" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.4">
@@ -12213,7 +12213,7 @@
         <v>102</v>
       </c>
       <c r="E111" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G111" t="s">
         <v>38</v>
@@ -12236,7 +12236,7 @@
         <v>102</v>
       </c>
       <c r="E112" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G112" t="s">
         <v>29</v>
@@ -12328,13 +12328,13 @@
         <v>77</v>
       </c>
       <c r="E116" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G116" t="s">
         <v>311</v>
       </c>
       <c r="I116" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.4">
@@ -12351,13 +12351,13 @@
         <v>77</v>
       </c>
       <c r="E117" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G117" t="s">
         <v>45</v>
       </c>
       <c r="I117" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.4">
@@ -12380,7 +12380,7 @@
         <v>79</v>
       </c>
       <c r="I118" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.4">
@@ -12426,7 +12426,7 @@
         <v>45</v>
       </c>
       <c r="I120" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.4">
@@ -12466,7 +12466,7 @@
         <v>79</v>
       </c>
       <c r="E122" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G122" t="s">
         <v>79</v>
@@ -12489,13 +12489,13 @@
         <v>79</v>
       </c>
       <c r="E123" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G123" t="s">
         <v>31</v>
       </c>
       <c r="I123" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.4">
@@ -12512,13 +12512,13 @@
         <v>79</v>
       </c>
       <c r="E124" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G124" t="s">
         <v>57</v>
       </c>
       <c r="I124" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.4">
@@ -12535,13 +12535,13 @@
         <v>79</v>
       </c>
       <c r="E125" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G125" t="s">
         <v>65</v>
       </c>
       <c r="I125" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.4">
@@ -12564,7 +12564,7 @@
         <v>44</v>
       </c>
       <c r="I126" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.4">
@@ -12581,7 +12581,7 @@
         <v>35</v>
       </c>
       <c r="E127" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G127" t="s">
         <v>13</v>
@@ -12621,7 +12621,7 @@
         <v>35</v>
       </c>
       <c r="E129" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G129" t="s">
         <v>45</v>
@@ -12641,7 +12641,7 @@
         <v>35</v>
       </c>
       <c r="E130" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G130" t="s">
         <v>22</v>
@@ -12664,7 +12664,7 @@
         <v>35</v>
       </c>
       <c r="E131" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G131" t="s">
         <v>31</v>
@@ -12687,13 +12687,13 @@
         <v>35</v>
       </c>
       <c r="E132" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G132" t="s">
         <v>38</v>
       </c>
       <c r="I132" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.4">
@@ -12710,7 +12710,7 @@
         <v>45</v>
       </c>
       <c r="E133" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G133" t="s">
         <v>120</v>
@@ -12733,7 +12733,7 @@
         <v>45</v>
       </c>
       <c r="E134" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G134" t="s">
         <v>33</v>
@@ -12779,13 +12779,13 @@
         <v>45</v>
       </c>
       <c r="E136" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G136" t="s">
         <v>57</v>
       </c>
       <c r="I136" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.4">
@@ -12802,13 +12802,13 @@
         <v>45</v>
       </c>
       <c r="E137" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G137" t="s">
         <v>46</v>
       </c>
       <c r="I137" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.4">
@@ -12825,13 +12825,13 @@
         <v>60</v>
       </c>
       <c r="E138" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="G138" t="s">
         <v>57</v>
       </c>
       <c r="I138" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.4">
@@ -12854,7 +12854,7 @@
         <v>22</v>
       </c>
       <c r="I139" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.4">
@@ -12877,7 +12877,7 @@
         <v>31</v>
       </c>
       <c r="I140" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.4">
@@ -12894,13 +12894,13 @@
         <v>120</v>
       </c>
       <c r="E141" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G141" t="s">
         <v>45</v>
       </c>
       <c r="I141" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.4">
@@ -12917,13 +12917,13 @@
         <v>120</v>
       </c>
       <c r="E142" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G142" t="s">
         <v>13</v>
       </c>
       <c r="I142" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.4">
@@ -12946,7 +12946,7 @@
         <v>14</v>
       </c>
       <c r="I143" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.4">
@@ -12963,13 +12963,13 @@
         <v>120</v>
       </c>
       <c r="E144" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G144" t="s">
         <v>31</v>
       </c>
       <c r="I144" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.4">
@@ -12986,13 +12986,13 @@
         <v>120</v>
       </c>
       <c r="E145" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G145" t="s">
         <v>46</v>
       </c>
       <c r="I145" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.4">
@@ -13015,7 +13015,7 @@
         <v>46</v>
       </c>
       <c r="I146" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.4">
@@ -13032,13 +13032,13 @@
         <v>120</v>
       </c>
       <c r="E147" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G147" t="s">
         <v>79</v>
       </c>
       <c r="I147" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.4">
@@ -13061,7 +13061,7 @@
         <v>79</v>
       </c>
       <c r="I148" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.4">
@@ -13078,13 +13078,13 @@
         <v>46</v>
       </c>
       <c r="E149" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G149" t="s">
         <v>22</v>
       </c>
       <c r="I149" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.4">
@@ -13101,7 +13101,7 @@
         <v>46</v>
       </c>
       <c r="E150" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G150" t="s">
         <v>64</v>
@@ -13144,7 +13144,7 @@
         <v>46</v>
       </c>
       <c r="E152" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G152" t="s">
         <v>171</v>
@@ -13173,7 +13173,7 @@
         <v>120</v>
       </c>
       <c r="I153" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.4">
@@ -13190,7 +13190,7 @@
         <v>46</v>
       </c>
       <c r="E154" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="G154" t="s">
         <v>22</v>
@@ -13213,7 +13213,7 @@
         <v>44</v>
       </c>
       <c r="E155" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="G155" t="s">
         <v>311</v>
@@ -13236,13 +13236,13 @@
         <v>44</v>
       </c>
       <c r="E156" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G156" t="s">
         <v>311</v>
       </c>
       <c r="I156" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.4">
@@ -13259,13 +13259,13 @@
         <v>44</v>
       </c>
       <c r="E157" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="G157" t="s">
         <v>311</v>
       </c>
       <c r="I157" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.4">
@@ -13282,7 +13282,7 @@
         <v>44</v>
       </c>
       <c r="E158" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G158" t="s">
         <v>3</v>
@@ -13305,13 +13305,13 @@
         <v>44</v>
       </c>
       <c r="E159" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G159" t="s">
         <v>3</v>
       </c>
       <c r="I159" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.4">
@@ -13328,7 +13328,7 @@
         <v>44</v>
       </c>
       <c r="E160" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="G160" t="s">
         <v>3</v>
@@ -13351,7 +13351,7 @@
         <v>65</v>
       </c>
       <c r="E161" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G161" t="s">
         <v>311</v>
@@ -13374,7 +13374,7 @@
         <v>65</v>
       </c>
       <c r="E162" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G162" t="s">
         <v>3</v>
@@ -13420,7 +13420,7 @@
         <v>65</v>
       </c>
       <c r="E164" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G164" t="s">
         <v>56</v>
@@ -13443,7 +13443,7 @@
         <v>65</v>
       </c>
       <c r="E165" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G165" t="s">
         <v>38</v>
@@ -13489,7 +13489,7 @@
         <v>14</v>
       </c>
       <c r="E167" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G167" t="s">
         <v>171</v>
@@ -13512,7 +13512,7 @@
         <v>14</v>
       </c>
       <c r="E168" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G168" t="s">
         <v>77</v>
@@ -13535,7 +13535,7 @@
         <v>14</v>
       </c>
       <c r="E169" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G169" t="s">
         <v>57</v>
@@ -13558,7 +13558,7 @@
         <v>14</v>
       </c>
       <c r="E170" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G170" t="s">
         <v>57</v>
@@ -13587,7 +13587,7 @@
         <v>57</v>
       </c>
       <c r="I171" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.4">
@@ -13610,7 +13610,7 @@
         <v>44</v>
       </c>
       <c r="I172" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.4">
@@ -13627,13 +13627,13 @@
         <v>311</v>
       </c>
       <c r="E173" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G173" t="s">
         <v>57</v>
       </c>
       <c r="I173" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.4">
@@ -13650,13 +13650,13 @@
         <v>311</v>
       </c>
       <c r="E174" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G174" t="s">
         <v>45</v>
       </c>
       <c r="I174" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.4">
@@ -13679,7 +13679,7 @@
         <v>38</v>
       </c>
       <c r="I175" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.4">
@@ -13696,13 +13696,13 @@
         <v>311</v>
       </c>
       <c r="E176" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G176" t="s">
         <v>29</v>
       </c>
       <c r="I176" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.4">
@@ -13719,13 +13719,13 @@
         <v>311</v>
       </c>
       <c r="E177" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G177" t="s">
         <v>119</v>
       </c>
       <c r="I177" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
   </sheetData>

</xml_diff>